<commit_message>
Fix Excel users loading with Vercel includeFiles and extra logging
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F714A1F2-1B61-45F0-AB04-C0276F6A0815}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A60CEDA-AD40-402E-AF41-B890CB6AA656}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,19 +37,19 @@
     <t>Іванов</t>
   </si>
   <si>
-    <t>pass123</t>
-  </si>
-  <si>
-    <t>pass456</t>
-  </si>
-  <si>
-    <t>pass789</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>adminpass</t>
+    <t>pass111</t>
+  </si>
+  <si>
+    <t>pass222</t>
+  </si>
+  <si>
+    <t>pass333</t>
+  </si>
+  <si>
+    <t>passadmin</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,7 +402,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -410,7 +410,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -418,12 +418,12 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Fix syntax in loadUsers and ensure server starts after loading users
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A60CEDA-AD40-402E-AF41-B890CB6AA656}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0A50B6-D9C1-475C-B674-0E0FABAEC3B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Петров</t>
-  </si>
-  <si>
     <t>Сідоров</t>
   </si>
   <si>
@@ -50,6 +47,9 @@
   </si>
   <si>
     <t>passadmin</t>
+  </si>
+  <si>
+    <t>user1</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,34 +399,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update users.xlsx with renamed sheet to Users and ensure file inclusion
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0A50B6-D9C1-475C-B674-0E0FABAEC3B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC412F84-E4BA-4018-B4FC-4769095FFD0E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,12 +28,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Сідоров</t>
-  </si>
-  <si>
-    <t>Іванов</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -50,6 +44,12 @@
   </si>
   <si>
     <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,34 +399,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update users.xlsx with new username and password
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC412F84-E4BA-4018-B4FC-4769095FFD0E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C7A4CA-6974-44F8-9614-F71552095CFE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,13 +43,13 @@
     <t>passadmin</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>user3</t>
+    <t>Іваненко</t>
+  </si>
+  <si>
+    <t>Петренко</t>
+  </si>
+  <si>
+    <t>Заічко</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>